<commit_message>
rerun with small cleans
added var with total persons (tot_pp)
</commit_message>
<xml_diff>
--- a/analyses/table_1_clean.xlsx
+++ b/analyses/table_1_clean.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\SNC_Swiss-SEP2\analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FDCF6F-B426-4599-B3F0-AFA5F1F1618F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105C81ED-A8F2-4792-9D85-C45E3E0DEF5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,36 +265,18 @@
     <t>49782 (48.6)</t>
   </si>
   <si>
-    <t>41660 (47.3)</t>
-  </si>
-  <si>
     <t>36229 (47.3)</t>
   </si>
   <si>
     <t>52601 (51.4)</t>
   </si>
   <si>
-    <t>46325 (52.7)</t>
-  </si>
-  <si>
-    <t>40309 (52.7)</t>
-  </si>
-  <si>
     <t>26569 (26.0)</t>
   </si>
   <si>
-    <t>20018 (22.8)</t>
-  </si>
-  <si>
-    <t>13510 (17.7)</t>
-  </si>
-  <si>
     <t>30416 (29.7)</t>
   </si>
   <si>
-    <t>25099 (28.5)</t>
-  </si>
-  <si>
     <t>21905 (28.6)</t>
   </si>
   <si>
@@ -331,9 +313,6 @@
     <t>50077 (56.9)</t>
   </si>
   <si>
-    <t>46283 (60.5)</t>
-  </si>
-  <si>
     <t>6156 (6.0)</t>
   </si>
   <si>
@@ -355,9 +334,6 @@
     <t>70681 (80.3)</t>
   </si>
   <si>
-    <t>62514 (81.7)</t>
-  </si>
-  <si>
     <t>32509 (31.8)</t>
   </si>
   <si>
@@ -370,12 +346,6 @@
     <t>40613 (39.7)</t>
   </si>
   <si>
-    <t>52825 (60.0)</t>
-  </si>
-  <si>
-    <t>53580 (70.0)</t>
-  </si>
-  <si>
     <t>34020 (33.2)</t>
   </si>
   <si>
@@ -388,9 +358,6 @@
     <t>12614 (12.3)</t>
   </si>
   <si>
-    <t>7659 (8.7)</t>
-  </si>
-  <si>
     <t>1355 (1.8)</t>
   </si>
   <si>
@@ -415,18 +382,9 @@
     <t>46845 (45.8)</t>
   </si>
   <si>
-    <t>45382 (51.6)</t>
-  </si>
-  <si>
-    <t>31333 (40.9)</t>
-  </si>
-  <si>
     <t>18306 (17.9)</t>
   </si>
   <si>
-    <t>23858 (27.1)</t>
-  </si>
-  <si>
     <t>39071 (51.0)</t>
   </si>
   <si>
@@ -451,9 +409,6 @@
     <t>3599 (3.5)</t>
   </si>
   <si>
-    <t>5233 (5.9)</t>
-  </si>
-  <si>
     <t>9250 (12.1)</t>
   </si>
   <si>
@@ -496,12 +451,6 @@
     <t>25702 (25.1)</t>
   </si>
   <si>
-    <t>22239 (25.3)</t>
-  </si>
-  <si>
-    <t>20098 (26.3)</t>
-  </si>
-  <si>
     <t>29395 (28.7)</t>
   </si>
   <si>
@@ -514,21 +463,12 @@
     <t>27683 (27.0)</t>
   </si>
   <si>
-    <t>22694 (25.8)</t>
-  </si>
-  <si>
     <t>26015 (34.0)</t>
   </si>
   <si>
     <t>30417 (29.7)</t>
   </si>
   <si>
-    <t>39056 (44.4)</t>
-  </si>
-  <si>
-    <t>49218 (64.3)</t>
-  </si>
-  <si>
     <t>44283 (43.3)</t>
   </si>
   <si>
@@ -536,6 +476,66 @@
   </si>
   <si>
     <t>1305 (1.7)</t>
+  </si>
+  <si>
+    <t>41659 (47.3)</t>
+  </si>
+  <si>
+    <t>46326 (52.7)</t>
+  </si>
+  <si>
+    <t>40308 (52.7)</t>
+  </si>
+  <si>
+    <t>20017 (22.8)</t>
+  </si>
+  <si>
+    <t>13509 (17.7)</t>
+  </si>
+  <si>
+    <t>25100 (28.5)</t>
+  </si>
+  <si>
+    <t>46282 (60.5)</t>
+  </si>
+  <si>
+    <t>62513 (81.7)</t>
+  </si>
+  <si>
+    <t>52824 (60.0)</t>
+  </si>
+  <si>
+    <t>53579 (70.0)</t>
+  </si>
+  <si>
+    <t>7660 (8.7)</t>
+  </si>
+  <si>
+    <t>45383 (51.6)</t>
+  </si>
+  <si>
+    <t>31332 (40.9)</t>
+  </si>
+  <si>
+    <t>23857 (27.1)</t>
+  </si>
+  <si>
+    <t>5232 (5.9)</t>
+  </si>
+  <si>
+    <t>22240 (25.3)</t>
+  </si>
+  <si>
+    <t>20097 (26.3)</t>
+  </si>
+  <si>
+    <t>22695 (25.8)</t>
+  </si>
+  <si>
+    <t>39055 (44.4)</t>
+  </si>
+  <si>
+    <t>49217 (64.3)</t>
   </si>
 </sst>
 </file>
@@ -579,7 +579,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -593,6 +593,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -935,7 +938,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:F35"/>
+      <selection activeCell="C15" sqref="C15:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -992,16 +995,16 @@
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1009,16 +1012,16 @@
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="C5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1029,16 +1032,16 @@
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="C6" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1046,16 +1049,16 @@
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="C7" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1063,16 +1066,16 @@
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="C8" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1080,16 +1083,16 @@
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="C9" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1100,16 +1103,16 @@
       <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="C10" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1117,16 +1120,16 @@
       <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="C11" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1134,16 +1137,16 @@
       <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F12" s="2" t="s">
+      <c r="C12" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1151,16 +1154,16 @@
       <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F13" s="2" t="s">
+      <c r="E13" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1168,16 +1171,16 @@
       <c r="B14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1188,16 +1191,16 @@
       <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F15" s="2" t="s">
+      <c r="C15" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1205,16 +1208,16 @@
       <c r="B16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F16" s="2" t="s">
+      <c r="C16" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1225,16 +1228,16 @@
       <c r="B17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F17" s="2" t="s">
+      <c r="C17" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1242,16 +1245,16 @@
       <c r="B18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F18" s="2" t="s">
+      <c r="C18" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1259,16 +1262,16 @@
       <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F19" s="2" t="s">
+      <c r="C19" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1276,16 +1279,16 @@
       <c r="B20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F20" s="2" t="s">
+      <c r="C20" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1296,16 +1299,16 @@
       <c r="B21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F21" s="2" t="s">
+      <c r="C21" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1313,16 +1316,16 @@
       <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F22" s="2" t="s">
+      <c r="C22" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1330,16 +1333,16 @@
       <c r="B23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F23" s="2" t="s">
+      <c r="C23" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F23" s="6" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1350,16 +1353,16 @@
       <c r="B24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F24" s="2" t="s">
+      <c r="C24" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1367,16 +1370,16 @@
       <c r="B25" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F25" s="2" t="s">
+      <c r="C25" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F25" s="6" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1384,16 +1387,16 @@
       <c r="B26" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F26" s="2" t="s">
+      <c r="C26" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F26" s="6" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1401,16 +1404,16 @@
       <c r="B27" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F27" s="2" t="s">
+      <c r="C27" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1418,16 +1421,16 @@
       <c r="B28" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F28" s="2" t="s">
+      <c r="C28" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1435,16 +1438,16 @@
       <c r="B29" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F29" s="2" t="s">
+      <c r="C29" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1452,16 +1455,16 @@
       <c r="B30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F30" s="2" t="s">
+      <c r="C30" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="F30" s="6" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1469,16 +1472,16 @@
       <c r="B31" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F31" s="2" t="s">
+      <c r="C31" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="F31" s="6" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1486,16 +1489,16 @@
       <c r="B32" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="F32" s="2" t="s">
+      <c r="C32" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="F32" s="6" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1506,16 +1509,16 @@
       <c r="B33" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="F33" s="2" t="s">
+      <c r="C33" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="F33" s="6" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1523,16 +1526,16 @@
       <c r="B34" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F34" s="2" t="s">
+      <c r="C34" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="F34" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1540,16 +1543,16 @@
       <c r="B35" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="F35" s="2" t="s">
+      <c r="C35" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>